<commit_message>
Added option to import in bulk
</commit_message>
<xml_diff>
--- a/data/excel/licenses.xlsx
+++ b/data/excel/licenses.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">icon</t>
   </si>
   <si>
-    <t xml:space="preserve">relatedURI_1</t>
+    <t xml:space="preserve">relatedURI_0</t>
   </si>
   <si>
     <t xml:space="preserve">CC</t>
@@ -804,8 +804,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>